<commit_message>
UI für Profil-Menü fertig
+ Styles-Klasse angepasst und Referenzen ebenfalls, Anpassungen an der USERS-Datenbank
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/d_aggarwal_sap_com/Documents/Duales Studium/HWG LU/Vorlesungen/2. Semester/Aktuelle Themen der IT/Repo/ATdIT_Gruppe5/databases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9898D139-E9CB-4F16-B4A1-A71061827F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{9898D139-E9CB-4F16-B4A1-A71061827F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89E0DA29-DF80-4FC7-B815-DC0991600046}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Max</t>
   </si>
@@ -160,16 +162,72 @@
   </si>
   <si>
     <t>role_id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>passwort123</t>
+  </si>
+  <si>
+    <t>max.mustermann@example.com</t>
+  </si>
+  <si>
+    <t>laura.koch@example.com</t>
+  </si>
+  <si>
+    <t>alex.schmidt@example.com</t>
+  </si>
+  <si>
+    <t>luisa.fuchs@example.com</t>
+  </si>
+  <si>
+    <t>robert.fischer@example.com</t>
+  </si>
+  <si>
+    <t>wolfgang.bauer@example.com</t>
+  </si>
+  <si>
+    <t>hermine.klein@example.com</t>
+  </si>
+  <si>
+    <t>steffanie.mueller@example.com</t>
+  </si>
+  <si>
+    <t>samuel.fischer@example.com</t>
+  </si>
+  <si>
+    <t>isLoggedIn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;;**"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -192,16 +250,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E69E-E720-4C2D-B81A-DEA44878441D}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,11 +594,13 @@
     <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="7" max="7" width="37" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -552,10 +620,19 @@
         <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -574,11 +651,20 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1">
         <v>1</v>
       </c>
+      <c r="J2" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -597,11 +683,20 @@
       <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1">
         <v>1</v>
       </c>
+      <c r="J3" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -620,11 +715,20 @@
       <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1">
         <v>1</v>
       </c>
+      <c r="J4" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -643,11 +747,20 @@
       <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1">
         <v>2</v>
       </c>
+      <c r="J5" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -666,11 +779,20 @@
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1">
         <v>1</v>
       </c>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -689,11 +811,20 @@
       <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1">
         <v>1</v>
       </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -712,11 +843,20 @@
       <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1">
         <v>2</v>
       </c>
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -735,11 +875,20 @@
       <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="1">
         <v>2</v>
       </c>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -758,12 +907,35 @@
       <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="1">
         <v>1</v>
+      </c>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6CCE9D38-E241-495E-B467-931EEDC3C12E}"/>
+    <hyperlink ref="G3:G10" r:id="rId2" display="max.mustermann@example.com" xr:uid="{077A01C1-E489-4149-B981-81DAB0D867CD}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{C11D9D94-AD0C-46DA-A6DD-3C7F0E2C9559}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{6EE26CD2-963C-4EF1-8815-7C2C179EE829}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{FCB8C551-BF70-49FF-9D6B-DAA9184AE13A}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{F8DF4196-CCE5-4419-94F0-56D0F89FFD88}"/>
+    <hyperlink ref="G7" r:id="rId7" xr:uid="{9282ADB0-F1C9-4E82-A032-E03E4D33CC5F}"/>
+    <hyperlink ref="G8" r:id="rId8" xr:uid="{78E4936E-6154-4676-B777-BB41E41CA510}"/>
+    <hyperlink ref="G9" r:id="rId9" xr:uid="{EB89BBE2-6BBC-4043-8778-02058B78B6E1}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{1CDB997A-7265-4C1F-896E-56EF5C692E03}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Obsolete "isAllowedToView" entfernt (auch aus Test)
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{9898D139-E9CB-4F16-B4A1-A71061827F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89E0DA29-DF80-4FC7-B815-DC0991600046}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85773E71-7F06-4F38-8AD9-CEA81A331D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -583,21 +583,22 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Errors sind beseitigt, DB Zellenformate modifiziert
+ weitere Methoden
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7BEE52-B642-4C3E-A843-00BE901B3409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{3D7BEE52-B642-4C3E-A843-00BE901B3409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E00D2D1-4013-4F9F-A8BB-34F094AB8AD7}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
+    <workbookView xWindow="-26880" yWindow="1920" windowWidth="21600" windowHeight="11430" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -284,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,7 +292,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -613,89 +619,89 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="A1:XFD1048576"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>77777</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="b">
@@ -703,34 +709,34 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>75196</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="b">
@@ -738,34 +744,34 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>68549</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>1</v>
       </c>
       <c r="K4" s="1" t="b">
@@ -773,34 +779,34 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>68775</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>2</v>
       </c>
       <c r="K5" s="1" t="b">
@@ -808,34 +814,34 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>71032</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>1</v>
       </c>
       <c r="K6" s="1" t="b">
@@ -843,34 +849,34 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>71065</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>1</v>
       </c>
       <c r="K7" s="1" t="b">
@@ -878,34 +884,34 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>74321</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>2</v>
       </c>
       <c r="K8" s="1" t="b">
@@ -913,34 +919,34 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>75172</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>2</v>
       </c>
       <c r="K9" s="1" t="b">
@@ -948,34 +954,34 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>75203</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>52</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="b">

</xml_diff>

<commit_message>
Excel-Extractor-Methoden fertig, parallel Tests geschrieben
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{3D7BEE52-B642-4C3E-A843-00BE901B3409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E00D2D1-4013-4F9F-A8BB-34F094AB8AD7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD8A89B-A090-4413-9BA2-9C53FA3545F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26880" yWindow="1920" windowWidth="21600" windowHeight="11430" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Max</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Laura</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>Steffanie</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>laura.koch@example.com</t>
   </si>
   <si>
-    <t>alex.schmidt@example.com</t>
-  </si>
-  <si>
     <t>luisa.fuchs@example.com</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>laura_koch</t>
   </si>
   <si>
-    <t>alex_schmidt</t>
-  </si>
-  <si>
     <t>steffanie_müller</t>
   </si>
   <si>
@@ -231,6 +222,12 @@
   </si>
   <si>
     <t>hermine_klein</t>
+  </si>
+  <si>
+    <t>max_schmidt</t>
+  </si>
+  <si>
+    <t>max.schmidt@example.com</t>
   </si>
 </sst>
 </file>
@@ -619,7 +616,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,37 +637,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -678,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -696,10 +693,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3">
         <v>1</v>
@@ -713,28 +710,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3">
         <v>75196</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
@@ -748,28 +745,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3">
         <v>68549</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -783,28 +780,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
         <v>68775</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -818,28 +815,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3">
         <v>71032</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
@@ -853,28 +850,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3">
         <v>71065</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
@@ -888,28 +885,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3">
         <v>74321</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" s="3">
         <v>2</v>
@@ -923,28 +920,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3">
         <v>75172</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J9" s="3">
         <v>2</v>
@@ -958,28 +955,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3">
         <v>75203</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Bug gefixed, Default-DBs hinzugefügt & in CAPS
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
   <si>
     <t>Max</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>max.schmidt@example.com</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Musterstraße 1</t>
   </si>
 </sst>
 </file>
@@ -621,18 +627,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="10.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="16.21875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="21.77734375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="32.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.21875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="7.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.21875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="11.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -671,8 +677,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>55</v>
@@ -684,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3">
-        <v>77777</v>
+        <v>66</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>12345.0</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>3</v>
@@ -698,8 +704,8 @@
       <c r="I2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="3">
-        <v>1</v>
+      <c r="J2" s="3" t="n">
+        <v>1.0</v>
       </c>
       <c r="K2" s="1" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update des WelcomeItems im UserMenu
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="68">
   <si>
     <t>Max</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Musterstraße 1</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Test-User angelegt für schnelles LogIn
</commit_message>
<xml_diff>
--- a/databases/Users.xlsx
+++ b/databases/Users.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I518185\OneDrive - SAP SE\Duales Studium\HWG LU\Vorlesungen\2. Semester\Aktuelle Themen der IT\Repo\ATdIT_Gruppe5\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD8A89B-A090-4413-9BA2-9C53FA3545F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6D070B-7619-4450-B756-8246D6506689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26880" yWindow="1920" windowWidth="21600" windowHeight="11430" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DD3FD198-26C0-4A6E-BD30-965DAB73A4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>Max</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Mustermann</t>
   </si>
   <si>
-    <t>Musterstraße 5</t>
-  </si>
-  <si>
     <t>Musterstadt</t>
   </si>
   <si>
@@ -230,13 +227,22 @@
     <t>max.schmidt@example.com</t>
   </si>
   <si>
-    <t>Ma</t>
-  </si>
-  <si>
     <t>Musterstraße 1</t>
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Teststraße 1</t>
+  </si>
+  <si>
+    <t>Teststadt</t>
+  </si>
+  <si>
+    <t>test.test@example.com</t>
   </si>
 </sst>
 </file>
@@ -290,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +311,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,69 +631,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A06E69E-E720-4C2D-B81A-DEA44878441D}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="13.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="10.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="13.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="16.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="8.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="21.77734375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="32.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.21875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="7.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="11.21875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="11.5546875" collapsed="true"/>
+    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.21875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="11.5546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="n">
-        <v>1.0</v>
+      <c r="A2" s="3">
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -693,22 +702,22 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>12345.0</v>
+        <v>64</v>
+      </c>
+      <c r="F2" s="3">
+        <v>12345</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>1.0</v>
+        <v>43</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="b">
         <v>0</v>
@@ -719,28 +728,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3">
         <v>75196</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
@@ -754,28 +763,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3">
         <v>68549</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -789,28 +798,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3">
         <v>68775</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
@@ -824,28 +833,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3">
         <v>71032</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="3">
         <v>1</v>
@@ -859,28 +868,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3">
         <v>71065</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
@@ -894,28 +903,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3">
         <v>74321</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" s="3">
         <v>2</v>
@@ -929,28 +938,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3">
         <v>75172</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="3">
         <v>2</v>
@@ -964,33 +973,68 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3">
         <v>75203</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="3">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1">
+        <v>77777</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1008,8 +1052,9 @@
     <hyperlink ref="H8" r:id="rId8" xr:uid="{78E4936E-6154-4676-B777-BB41E41CA510}"/>
     <hyperlink ref="H9" r:id="rId9" xr:uid="{EB89BBE2-6BBC-4043-8778-02058B78B6E1}"/>
     <hyperlink ref="H10" r:id="rId10" xr:uid="{1CDB997A-7265-4C1F-896E-56EF5C692E03}"/>
+    <hyperlink ref="H11" r:id="rId11" xr:uid="{388FFC9E-932B-430E-8A59-19D659C4A1A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>